<commit_message>
Update country data files
</commit_message>
<xml_diff>
--- a/assets/data/MSME Country Indicators - Afghanistan Summary.xlsx
+++ b/assets/data/MSME Country Indicators - Afghanistan Summary.xlsx
@@ -5,13 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Summary" sheetId="1" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -19,6 +19,9 @@
     <t>MSME Participation on the Economy</t>
   </si>
   <si>
+    <t>Source Type: SME Associations (Most Widely Used)</t>
+  </si>
+  <si>
     <t>Micro</t>
   </si>
   <si>
@@ -28,6 +31,12 @@
     <t>MSMEs</t>
   </si>
   <si>
+    <t>Employment (% of total)</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>Enterprises (% of total)</t>
   </si>
   <si>
@@ -35,6 +44,12 @@
   </si>
   <si>
     <t>Source: MFA, 2010</t>
+  </si>
+  <si>
+    <t>MFA</t>
+  </si>
+  <si>
+    <t>Ministry of Foreign Affaris (MFA), "SMALL TO MEDIUM ENTERPRISE PAPERS", N/S, p. 3. Available at http://mfa.gov.af/content/files/SME%20PAPER.pdf</t>
   </si>
 </sst>
 </file>
@@ -42,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -53,6 +68,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -85,26 +106,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="0" fontId="1"/>
     <xf numFmtId="0" fontId="2"/>
     <xf numFmtId="0" fontId="3"/>
     <xf numFmtId="0" fontId="4"/>
+    <xf numFmtId="0" fontId="5"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="2"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="3"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" xfId="4"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="name" xfId="1"/>
     <cellStyle name="title" xfId="2"/>
-    <cellStyle name="source" xfId="3"/>
-    <cellStyle name="HyperLink" xfId="4"/>
+    <cellStyle name="title_" xfId="3"/>
+    <cellStyle name="source" xfId="4"/>
+    <cellStyle name="HyperLink" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -112,7 +136,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -128,28 +152,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
+    <row r="9">
+      <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="D12" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>